<commit_message>
added code to import data from excel file
reformat DataFrames to Arrays/Dicts where needed
</commit_message>
<xml_diff>
--- a/test/left-right.xlsx
+++ b/test/left-right.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="973" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Commodity" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>Site</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Commodity</t>
   </si>
   <si>
-    <t>price</t>
+    <t>Price</t>
   </si>
   <si>
     <t>Left</t>
@@ -43,10 +43,22 @@
     <t>Right</t>
   </si>
   <si>
+    <t>Magic</t>
+  </si>
+  <si>
     <t>Process</t>
   </si>
   <si>
+    <t>MinOut</t>
+  </si>
+  <si>
+    <t>MaxOut</t>
+  </si>
+  <si>
     <t>Coal plant</t>
+  </si>
+  <si>
+    <t>Mage</t>
   </si>
   <si>
     <t>Direction</t>
@@ -79,6 +91,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -160,16 +173,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -202,6 +212,17 @@
       </c>
       <c r="C3" s="0" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -220,23 +241,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,21 +268,47 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>7</v>
+    </row>
+    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -271,40 +321,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -312,22 +359,50 @@
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -347,13 +422,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>3</v>
@@ -409,7 +481,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
add capacity increase and pricing information to processes
additional columns in excel sheet
more fields in Process-type
costs now also include variable/fix/investment costs
adjust tests
</commit_message>
<xml_diff>
--- a/test/left-right.xlsx
+++ b/test/left-right.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Commodity" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Site</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Commodity</t>
   </si>
   <si>
-    <t>Price</t>
+    <t>price</t>
   </si>
   <si>
     <t>Left</t>
@@ -49,10 +49,22 @@
     <t>Process</t>
   </si>
   <si>
-    <t>MinOut</t>
-  </si>
-  <si>
-    <t>MaxOut</t>
+    <t>inst-cap</t>
+  </si>
+  <si>
+    <t>cap-lo</t>
+  </si>
+  <si>
+    <t>cap-up</t>
+  </si>
+  <si>
+    <t>fix-cost</t>
+  </si>
+  <si>
+    <t>var-cost</t>
+  </si>
+  <si>
+    <t>inv-cost</t>
   </si>
   <si>
     <t>Coal plant</t>
@@ -151,8 +163,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -175,53 +191,58 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>5</v>
       </c>
     </row>
@@ -241,68 +262,119 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="n">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>1000</v>
       </c>
+      <c r="F2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="F3" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="0" t="n">
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>1000</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -328,74 +400,77 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>13</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="0" t="n">
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="0" t="n">
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -422,59 +497,62 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="B4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjusting to urbs excel-format
rename and add missing columns
</commit_message>
<xml_diff>
--- a/test/left-right.xlsx
+++ b/test/left-right.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Commodity" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>Site</t>
   </si>
@@ -31,6 +31,9 @@
     <t>Commodity</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
     <t>price</t>
   </si>
   <si>
@@ -40,6 +43,9 @@
     <t>Coal</t>
   </si>
   <si>
+    <t>Stock</t>
+  </si>
+  <si>
     <t>Right</t>
   </si>
   <si>
@@ -89,6 +95,12 @@
   </si>
   <si>
     <t>t</t>
+  </si>
+  <si>
+    <t>Left.Elec</t>
+  </si>
+  <si>
+    <t>Right.Elec</t>
   </si>
 </sst>
 </file>
@@ -189,17 +201,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -212,37 +222,49 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="D4" s="1" t="n">
         <v>5</v>
       </c>
     </row>
@@ -264,47 +286,44 @@
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0</v>
@@ -327,10 +346,10 @@
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -353,10 +372,10 @@
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0</v>
@@ -400,33 +419,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
@@ -434,13 +450,13 @@
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
@@ -448,13 +464,13 @@
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
@@ -462,13 +478,13 @@
     </row>
     <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
@@ -493,23 +509,20 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added natural resources to excelsheet
</commit_message>
<xml_diff>
--- a/test/left-right.xlsx
+++ b/test/left-right.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Commodity" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Process" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Process-Commodity" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Demand" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="SupIm" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,84 +24,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
-  <si>
-    <t>Site</t>
-  </si>
-  <si>
-    <t>Commodity</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>Left</t>
-  </si>
-  <si>
-    <t>Coal</t>
-  </si>
-  <si>
-    <t>Stock</t>
-  </si>
-  <si>
-    <t>Right</t>
-  </si>
-  <si>
-    <t>Magic</t>
-  </si>
-  <si>
-    <t>Process</t>
-  </si>
-  <si>
-    <t>inst-cap</t>
-  </si>
-  <si>
-    <t>cap-lo</t>
-  </si>
-  <si>
-    <t>cap-up</t>
-  </si>
-  <si>
-    <t>fix-cost</t>
-  </si>
-  <si>
-    <t>var-cost</t>
-  </si>
-  <si>
-    <t>inv-cost</t>
-  </si>
-  <si>
-    <t>Coal plant</t>
-  </si>
-  <si>
-    <t>Mage</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>ratio</t>
-  </si>
-  <si>
-    <t>in</t>
-  </si>
-  <si>
-    <t>Elec</t>
-  </si>
-  <si>
-    <t>out</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>Left.Elec</t>
-  </si>
-  <si>
-    <t>Right.Elec</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+  <si>
+    <t xml:space="preserve">Site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commodity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SupIm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inst-cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cap-lo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cap-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix-cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var-cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inv-cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coal plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waterplant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WaterplantElec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left.Elec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right.Elec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right.Water</t>
   </si>
 </sst>
 </file>
@@ -108,7 +124,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -201,15 +217,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -266,6 +284,21 @@
       </c>
       <c r="D4" s="1" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="0" t="e">
+        <f aca="false">NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -284,38 +317,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -323,7 +359,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0</v>
@@ -349,7 +385,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -375,7 +411,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0</v>
@@ -393,6 +429,32 @@
         <v>0.5</v>
       </c>
       <c r="H4" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="0" t="n">
         <v>10</v>
       </c>
     </row>
@@ -412,37 +474,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
@@ -450,13 +515,13 @@
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
@@ -464,13 +529,13 @@
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
@@ -478,15 +543,40 @@
     </row>
     <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -513,16 +603,19 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,6 +660,73 @@
       </c>
       <c r="C5" s="1" t="n">
         <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
split process throughput into 3 vars + fix math
throughput now = com_in -> pro_through -> com_out
switched side of process commodity ratios to pro_through
fixed excelfile
</commit_message>
<xml_diff>
--- a/test/left-right.xlsx
+++ b/test/left-right.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Commodity" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t xml:space="preserve">Site</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t xml:space="preserve">out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WaterplantElec</t>
   </si>
   <si>
     <t xml:space="preserve">t</t>
@@ -225,9 +222,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -319,13 +316,13 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,13 +473,13 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,7 +568,10 @@
     </row>
     <row r="7" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>25</v>
@@ -604,18 +604,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,16 +685,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added transmission to excelfile + adapt test
</commit_message>
<xml_diff>
--- a/test/left-right.xlsx
+++ b/test/left-right.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Commodity" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Process" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Process-Commodity" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Demand" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="SupIm" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Transmission" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Demand" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="SupIm" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
   <si>
     <t xml:space="preserve">Site</t>
   </si>
@@ -102,6 +103,24 @@
   </si>
   <si>
     <t xml:space="preserve">out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wacc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">depreciation</t>
   </si>
   <si>
     <t xml:space="preserve">t</t>
@@ -217,14 +236,12 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,13 +334,10 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -391,7 +405,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>5</v>
@@ -473,14 +487,11 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -596,70 +607,91 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>28</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="n">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>11</v>
+      <c r="L2" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -678,6 +710,85 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -685,13 +796,16 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
adjust excel to storage
</commit_message>
<xml_diff>
--- a/test/left-right.xlsx
+++ b/test/left-right.xlsx
@@ -5,15 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Commodity" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Process" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Process-Commodity" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Transmission" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Demand" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="SupIm" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Storage" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Demand" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="SupIm" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,114 +26,168 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
-  <si>
-    <t xml:space="preserve">Site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commodity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SupIm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inst-cap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cap-lo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cap-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fix-cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">var-cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inv-cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coal plant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waterplant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site In</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site Out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transmission</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wacc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">depreciation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Left.Elec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Right.Elec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Right.Water</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Commodity</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Magic</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>SupIm</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>inst-cap</t>
+  </si>
+  <si>
+    <t>cap-lo</t>
+  </si>
+  <si>
+    <t>cap-up</t>
+  </si>
+  <si>
+    <t>fix-cost</t>
+  </si>
+  <si>
+    <t>var-cost</t>
+  </si>
+  <si>
+    <t>inv-cost</t>
+  </si>
+  <si>
+    <t>Coal plant</t>
+  </si>
+  <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>Waterplant</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>Elec</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>Site In</t>
+  </si>
+  <si>
+    <t>Site Out</t>
+  </si>
+  <si>
+    <t>Transmission</t>
+  </si>
+  <si>
+    <t>eff</t>
+  </si>
+  <si>
+    <t>wacc</t>
+  </si>
+  <si>
+    <t>depreciation</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>inst-cap-c</t>
+  </si>
+  <si>
+    <t>cap-lo-c</t>
+  </si>
+  <si>
+    <t>cap-up-c</t>
+  </si>
+  <si>
+    <t>inst-cap-p</t>
+  </si>
+  <si>
+    <t>cap-lo-p</t>
+  </si>
+  <si>
+    <t>cap-up-p</t>
+  </si>
+  <si>
+    <t>eff-in</t>
+  </si>
+  <si>
+    <t>eff-out</t>
+  </si>
+  <si>
+    <t>inv-cost-p</t>
+  </si>
+  <si>
+    <t>inv-cost-c</t>
+  </si>
+  <si>
+    <t>fix-cost-p</t>
+  </si>
+  <si>
+    <t>fix-cost-c</t>
+  </si>
+  <si>
+    <t>var-cost-p</t>
+  </si>
+  <si>
+    <t>var-cost-c</t>
+  </si>
+  <si>
+    <t>init</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>inf</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>Left.Elec</t>
+  </si>
+  <si>
+    <t>Right.Elec</t>
+  </si>
+  <si>
+    <t>Right.Water</t>
   </si>
 </sst>
 </file>
@@ -140,7 +195,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -241,7 +296,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,11 +390,14 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -405,7 +465,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>5</v>
@@ -492,6 +552,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -609,14 +672,11 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -710,6 +770,151 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -717,16 +922,19 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -784,7 +992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -797,15 +1005,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>